<commit_message>
fix polarity of LED
</commit_message>
<xml_diff>
--- a/99_Resources/python/XlateURLsForStandAlone.xlsx
+++ b/99_Resources/python/XlateURLsForStandAlone.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FC9F6E-6E72-4D33-9BF2-52472154A508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6276DFC2-15CE-48FC-87D1-1D15B78591C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{8ED520A1-9624-40EB-A0BD-451A4B57B1C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{8ED520A1-9624-40EB-A0BD-451A4B57B1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2058,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C540BD1-6218-4126-83E7-AFCE5D23BAAF}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:D69"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4213,7 +4213,7 @@
         <f>LEN(B60)</f>
         <v>38</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>247</v>
       </c>
       <c r="C60" t="s">
@@ -4540,9 +4540,10 @@
     <hyperlink ref="B50" r:id="rId1" xr:uid="{EB67CE3E-1E20-49CF-B57E-A0AF5AE40E6E}"/>
     <hyperlink ref="B58" r:id="rId2" xr:uid="{8B47E7AD-D542-4FFF-AE7B-26337C515F0D}"/>
     <hyperlink ref="B45" r:id="rId3" xr:uid="{41D65414-9954-4D0F-A9F3-817162AA9DDA}"/>
+    <hyperlink ref="B60" r:id="rId4" xr:uid="{39FA7108-7901-4714-B768-69CEFE730CB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -4550,7 +4551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBCAD21-0F7B-4758-92D6-6CB5F17FACC1}">
   <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mostly documentation updates to htmlcomplete_to_good.py
</commit_message>
<xml_diff>
--- a/99_Resources/python/XlateURLsForStandAlone.xlsx
+++ b/99_Resources/python/XlateURLsForStandAlone.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5CC958-ACDE-4BC0-84D3-92FB6ED6DF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D9AB62-0268-488F-AC0D-DB2B7566B4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="6210" windowWidth="24825" windowHeight="12255" activeTab="3" xr2:uid="{8ED520A1-9624-40EB-A0BD-451A4B57B1C7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="313">
   <si>
     <t>2021-10-07_Library_from_googleusercontent.com.jpg</t>
   </si>
@@ -954,6 +954,18 @@
   </si>
   <si>
     <t>PDF/PNG/JPG</t>
+  </si>
+  <si>
+    <t>https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/01_Blink/01_Blink.ino</t>
+  </si>
+  <si>
+    <t>ArduinoCode/01_Blink/01_Blink.ino</t>
+  </si>
+  <si>
+    <t>ArduinoCode/02_LetsGetTalking/02_LetsGetTalking.ino</t>
+  </si>
+  <si>
+    <t>ArduinoCode/03_YakityYak/03_YakityYak.ino</t>
   </si>
 </sst>
 </file>
@@ -1038,12 +1050,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4916,10 +4931,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552D0541-A209-4C66-8ADB-AB8FD7A1A45E}">
-  <dimension ref="A2:K39"/>
+  <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4996,7 +5011,7 @@
         <f>IF(0=SUM(E3:G3),1,0)</f>
         <v>0</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J3" s="6" t="str">
         <f>IF(E3+F3,MID(D3,1+FIND("/",D3),999),IF(G3&gt;0,SUBSTITUTE(SUBSTITUTE(D3,"/README.md",".html"),"/","_"),SUBSTITUTE(D3,"/","_")&amp;".html"))</f>
         <v>Images/Arduino-Nano-Pinout_from_circuitstoday.com.png</v>
       </c>
@@ -5037,12 +5052,12 @@
         <f>IF(0=SUM(E4:G4),1,0)</f>
         <v>0</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J4" s="6" t="str">
         <f>IF(E4+F4,MID(D4,1+FIND("/",D4),999),IF(G4&gt;0,SUBSTITUTE(SUBSTITUTE(D4,"/README.md",".html"),"/","_"),SUBSTITUTE(D4,"/","_")&amp;".html"))</f>
         <v>02_LetsGetTalking.html#ascii-characters-and-strings</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K39" si="0">"    ["""&amp;B4&amp;""", """&amp;J4&amp;"""],"</f>
+        <f>"    ["""&amp;B4&amp;""", """&amp;J4&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/02_LetsGetTalking/README.md#ascii-characters-and-strings", "02_LetsGetTalking.html#ascii-characters-and-strings"],</v>
       </c>
     </row>
@@ -5055,35 +5070,35 @@
         <v>273</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C39" si="1">FIND("master/",B5)+LEN("master")+1</f>
+        <f>FIND("master/",B5)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5:D39" si="2">MID(B5,C5,9999)</f>
+        <f>MID(B5,C5,9999)</f>
         <v>99_Resources/Images/Config_USB_SerialMonitor_screen.png</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E39" si="3">COUNTIF($D5,"*.png*")+COUNTIF($D5,"*.jpg*")+COUNTIF($D5,"*.pdf*")</f>
+        <f>COUNTIF($D5,"*.png*")+COUNTIF($D5,"*.jpg*")+COUNTIF($D5,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F39" si="4">IF(COUNTIF($D5,"*.xls*"),1,0)</f>
+        <f>IF(COUNTIF($D5,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G39" si="5">IF(COUNTIF($D5,"*.md*"),1,0)</f>
+        <f>IF(COUNTIF($D5,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H39" si="6">IF(0=SUM(E5:G5),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" ref="J5:J39" si="7">IF(E5+F5,MID(D5,1+FIND("/",D5),999),IF(G5&gt;0,SUBSTITUTE(SUBSTITUTE(D5,"/README.md",".html"),"/","_"),SUBSTITUTE(D5,"/","_")&amp;".html"))</f>
+        <f>IF(0=SUM(E5:G5),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="6" t="str">
+        <f>IF(E5+F5,MID(D5,1+FIND("/",D5),999),IF(G5&gt;0,SUBSTITUTE(SUBSTITUTE(D5,"/README.md",".html"),"/","_"),SUBSTITUTE(D5,"/","_")&amp;".html"))</f>
         <v>Images/Config_USB_SerialMonitor_screen.png</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B5&amp;""", """&amp;J5&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/Config_USB_SerialMonitor_screen.png", "Images/Config_USB_SerialMonitor_screen.png"],</v>
       </c>
     </row>
@@ -5096,35 +5111,35 @@
         <v>274</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B6)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B6,C6,9999)</f>
         <v>99_Resources/Images/03_SerMon_DO_DEBUG_INPUT_run.png</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D6,"*.png*")+COUNTIF($D6,"*.jpg*")+COUNTIF($D6,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D6,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D6,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(0=SUM(E6:G6),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="6" t="str">
+        <f>IF(E6+F6,MID(D6,1+FIND("/",D6),999),IF(G6&gt;0,SUBSTITUTE(SUBSTITUTE(D6,"/README.md",".html"),"/","_"),SUBSTITUTE(D6,"/","_")&amp;".html"))</f>
         <v>Images/03_SerMon_DO_DEBUG_INPUT_run.png</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B6&amp;""", """&amp;J6&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/03_SerMon_DO_DEBUG_INPUT_run.png", "Images/03_SerMon_DO_DEBUG_INPUT_run.png"],</v>
       </c>
     </row>
@@ -5137,35 +5152,35 @@
         <v>275</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B7)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B7,C7,9999)</f>
         <v>99_Resources/Images/01_BlinkingLED_part_A_setup.png</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D7,"*.png*")+COUNTIF($D7,"*.jpg*")+COUNTIF($D7,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D7,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D7,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(0=SUM(E7:G7),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="6" t="str">
+        <f>IF(E7+F7,MID(D7,1+FIND("/",D7),999),IF(G7&gt;0,SUBSTITUTE(SUBSTITUTE(D7,"/README.md",".html"),"/","_"),SUBSTITUTE(D7,"/","_")&amp;".html"))</f>
         <v>Images/01_BlinkingLED_part_A_setup.png</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B7&amp;""", """&amp;J7&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/01_BlinkingLED_part_A_setup.png", "Images/01_BlinkingLED_part_A_setup.png"],</v>
       </c>
     </row>
@@ -5174,40 +5189,15 @@
         <f>LEN(B8)</f>
         <v>110</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>276</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="2"/>
-        <v>ArduinoCode/02_LetsGetTalking/02_LetsGetTalking.ino</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="7"/>
-        <v>ArduinoCode_02_LetsGetTalking_02_LetsGetTalking.ino.html</v>
+      <c r="J8" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/02_LetsGetTalking/02_LetsGetTalking.ino", "ArduinoCode_02_LetsGetTalking_02_LetsGetTalking.ino.html"],</v>
+        <f>"    ["""&amp;B8&amp;""", """&amp;J8&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/02_LetsGetTalking/02_LetsGetTalking.ino", "ArduinoCode/02_LetsGetTalking/02_LetsGetTalking.ino"],</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5219,35 +5209,35 @@
         <v>277</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B9)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B9,C9,9999)</f>
         <v>99_Resources/Images/Config_USB_SerialMonitor.png</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D9,"*.png*")+COUNTIF($D9,"*.jpg*")+COUNTIF($D9,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D9,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D9,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E9:G9),1,0)</f>
         <v>0</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E9+F9,MID(D9,1+FIND("/",D9),999),IF(G9&gt;0,SUBSTITUTE(SUBSTITUTE(D9,"/README.md",".html"),"/","_"),SUBSTITUTE(D9,"/","_")&amp;".html"))</f>
         <v>Images/Config_USB_SerialMonitor.png</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B9&amp;""", """&amp;J9&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/Config_USB_SerialMonitor.png", "Images/Config_USB_SerialMonitor.png"],</v>
       </c>
     </row>
@@ -5260,35 +5250,35 @@
         <v>278</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B10)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B10,C10,9999)</f>
         <v>99_Resources/Images/03_SerMon_DO_DEBUG_run.png</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D10,"*.png*")+COUNTIF($D10,"*.jpg*")+COUNTIF($D10,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D10,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D10,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E10:G10),1,0)</f>
         <v>0</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E10+F10,MID(D10,1+FIND("/",D10),999),IF(G10&gt;0,SUBSTITUTE(SUBSTITUTE(D10,"/README.md",".html"),"/","_"),SUBSTITUTE(D10,"/","_")&amp;".html"))</f>
         <v>Images/03_SerMon_DO_DEBUG_run.png</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B10&amp;""", """&amp;J10&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/03_SerMon_DO_DEBUG_run.png", "Images/03_SerMon_DO_DEBUG_run.png"],</v>
       </c>
     </row>
@@ -5301,35 +5291,35 @@
         <v>279</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B11)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B11,C11,9999)</f>
         <v>99_Resources/Images/02_SerMon_setup_only.png</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D11,"*.png*")+COUNTIF($D11,"*.jpg*")+COUNTIF($D11,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D11,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D11,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E11:G11),1,0)</f>
         <v>0</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E11+F11,MID(D11,1+FIND("/",D11),999),IF(G11&gt;0,SUBSTITUTE(SUBSTITUTE(D11,"/README.md",".html"),"/","_"),SUBSTITUTE(D11,"/","_")&amp;".html"))</f>
         <v>Images/02_SerMon_setup_only.png</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B11&amp;""", """&amp;J11&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/02_SerMon_setup_only.png", "Images/02_SerMon_setup_only.png"],</v>
       </c>
     </row>
@@ -5342,35 +5332,35 @@
         <v>280</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B12)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B12,C12,9999)</f>
         <v>99_Resources/Images/IDE_CompileAndRun.png</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D12,"*.png*")+COUNTIF($D12,"*.jpg*")+COUNTIF($D12,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D12,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D12,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E12:G12),1,0)</f>
         <v>0</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E12+F12,MID(D12,1+FIND("/",D12),999),IF(G12&gt;0,SUBSTITUTE(SUBSTITUTE(D12,"/README.md",".html"),"/","_"),SUBSTITUTE(D12,"/","_")&amp;".html"))</f>
         <v>Images/IDE_CompileAndRun.png</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B12&amp;""", """&amp;J12&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/IDE_CompileAndRun.png", "Images/IDE_CompileAndRun.png"],</v>
       </c>
     </row>
@@ -5379,40 +5369,15 @@
         <f>LEN(B13)</f>
         <v>100</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>281</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>ArduinoCode/03_YakityYak/03_YakityYak.ino</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="7"/>
-        <v>ArduinoCode_03_YakityYak_03_YakityYak.ino.html</v>
+      <c r="J13" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/03_YakityYak/03_YakityYak.ino", "ArduinoCode_03_YakityYak_03_YakityYak.ino.html"],</v>
+        <f>"    ["""&amp;B13&amp;""", """&amp;J13&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/03_YakityYak/03_YakityYak.ino", "ArduinoCode/03_YakityYak/03_YakityYak.ino"],</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -5424,35 +5389,35 @@
         <v>282</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B14)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B14,C14,9999)</f>
         <v>ArduinoCode/02_LetsGetTalking/README.md</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D14,"*.png*")+COUNTIF($D14,"*.jpg*")+COUNTIF($D14,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D14,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D14,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H14">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E14:G14),1,0)</f>
         <v>0</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E14+F14,MID(D14,1+FIND("/",D14),999),IF(G14&gt;0,SUBSTITUTE(SUBSTITUTE(D14,"/README.md",".html"),"/","_"),SUBSTITUTE(D14,"/","_")&amp;".html"))</f>
         <v>ArduinoCode_02_LetsGetTalking.html</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B14&amp;""", """&amp;J14&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/02_LetsGetTalking/README.md", "ArduinoCode_02_LetsGetTalking.html"],</v>
       </c>
     </row>
@@ -5465,35 +5430,35 @@
         <v>283</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B15)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B15,C15,9999)</f>
         <v>ArduinoCode/02_LetsGetTalking/README.md</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D15,"*.png*")+COUNTIF($D15,"*.jpg*")+COUNTIF($D15,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D15,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D15,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H15">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E15:G15),1,0)</f>
         <v>0</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E15+F15,MID(D15,1+FIND("/",D15),999),IF(G15&gt;0,SUBSTITUTE(SUBSTITUTE(D15,"/README.md",".html"),"/","_"),SUBSTITUTE(D15,"/","_")&amp;".html"))</f>
         <v>ArduinoCode_02_LetsGetTalking.html</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B15&amp;""", """&amp;J15&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/ArduinoCode/02_LetsGetTalking/README.md", "ArduinoCode_02_LetsGetTalking.html"],</v>
       </c>
     </row>
@@ -5506,35 +5471,35 @@
         <v>284</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B16)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B16,C16,9999)</f>
         <v>99_Resources/Images/02_SerMon_run.png</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D16,"*.png*")+COUNTIF($D16,"*.jpg*")+COUNTIF($D16,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D16,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D16,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E16:G16),1,0)</f>
         <v>0</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E16+F16,MID(D16,1+FIND("/",D16),999),IF(G16&gt;0,SUBSTITUTE(SUBSTITUTE(D16,"/README.md",".html"),"/","_"),SUBSTITUTE(D16,"/","_")&amp;".html"))</f>
         <v>Images/02_SerMon_run.png</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B16&amp;""", """&amp;J16&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/02_SerMon_run.png", "Images/02_SerMon_run.png"],</v>
       </c>
     </row>
@@ -5547,35 +5512,35 @@
         <v>285</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B17)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B17,C17,9999)</f>
         <v>99_Resources/Images/03_SerMon_run.png</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D17,"*.png*")+COUNTIF($D17,"*.jpg*")+COUNTIF($D17,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D17,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D17,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E17:G17),1,0)</f>
         <v>0</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E17+F17,MID(D17,1+FIND("/",D17),999),IF(G17&gt;0,SUBSTITUTE(SUBSTITUTE(D17,"/README.md",".html"),"/","_"),SUBSTITUTE(D17,"/","_")&amp;".html"))</f>
         <v>Images/03_SerMon_run.png</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B17&amp;""", """&amp;J17&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/03_SerMon_run.png", "Images/03_SerMon_run.png"],</v>
       </c>
     </row>
@@ -5588,35 +5553,35 @@
         <v>286</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B18)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B18,C18,9999)</f>
         <v>99_Resources/Images/IDE_LoadBlink.png</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D18,"*.png*")+COUNTIF($D18,"*.jpg*")+COUNTIF($D18,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D18,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D18,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E18:G18),1,0)</f>
         <v>0</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E18+F18,MID(D18,1+FIND("/",D18),999),IF(G18&gt;0,SUBSTITUTE(SUBSTITUTE(D18,"/README.md",".html"),"/","_"),SUBSTITUTE(D18,"/","_")&amp;".html"))</f>
         <v>Images/IDE_LoadBlink.png</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B18&amp;""", """&amp;J18&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/IDE_LoadBlink.png", "Images/IDE_LoadBlink.png"],</v>
       </c>
     </row>
@@ -5629,35 +5594,35 @@
         <v>287</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B19)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B19,C19,9999)</f>
         <v>README.md#some-resources-on-the-web</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D19,"*.png*")+COUNTIF($D19,"*.jpg*")+COUNTIF($D19,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D19,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D19,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H19">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E19:G19),1,0)</f>
         <v>0</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E19+F19,MID(D19,1+FIND("/",D19),999),IF(G19&gt;0,SUBSTITUTE(SUBSTITUTE(D19,"/README.md",".html"),"/","_"),SUBSTITUTE(D19,"/","_")&amp;".html"))</f>
         <v>README.md#some-resources-on-the-web</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B19&amp;""", """&amp;J19&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/README.md#some-resources-on-the-web", "README.md#some-resources-on-the-web"],</v>
       </c>
     </row>
@@ -5670,35 +5635,35 @@
         <v>288</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B20)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B20,C20,9999)</f>
         <v>ArduinoCode/03_YakityYak/README.md</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D20,"*.png*")+COUNTIF($D20,"*.jpg*")+COUNTIF($D20,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D20,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D20,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H20">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E20:G20),1,0)</f>
         <v>0</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E20+F20,MID(D20,1+FIND("/",D20),999),IF(G20&gt;0,SUBSTITUTE(SUBSTITUTE(D20,"/README.md",".html"),"/","_"),SUBSTITUTE(D20,"/","_")&amp;".html"))</f>
         <v>ArduinoCode_03_YakityYak.html</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B20&amp;""", """&amp;J20&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/03_YakityYak/README.md", "ArduinoCode_03_YakityYak.html"],</v>
       </c>
     </row>
@@ -5711,35 +5676,35 @@
         <v>289</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B21)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B21,C21,9999)</f>
         <v>99_Resources/Images/ConfigUSB.png</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D21,"*.png*")+COUNTIF($D21,"*.jpg*")+COUNTIF($D21,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D21,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D21,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E21:G21),1,0)</f>
         <v>0</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E21+F21,MID(D21,1+FIND("/",D21),999),IF(G21&gt;0,SUBSTITUTE(SUBSTITUTE(D21,"/README.md",".html"),"/","_"),SUBSTITUTE(D21,"/","_")&amp;".html"))</f>
         <v>Images/ConfigUSB.png</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B21&amp;""", """&amp;J21&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/ConfigUSB.png", "Images/ConfigUSB.png"],</v>
       </c>
     </row>
@@ -5752,35 +5717,35 @@
         <v>290</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B22)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B22,C22,9999)</f>
         <v>99_Resources/Images/IDE_Blink.png</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D22,"*.png*")+COUNTIF($D22,"*.jpg*")+COUNTIF($D22,"*.pdf*")</f>
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D22,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D22,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E22:G22),1,0)</f>
         <v>0</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E22+F22,MID(D22,1+FIND("/",D22),999),IF(G22&gt;0,SUBSTITUTE(SUBSTITUTE(D22,"/README.md",".html"),"/","_"),SUBSTITUTE(D22,"/","_")&amp;".html"))</f>
         <v>Images/IDE_Blink.png</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B22&amp;""", """&amp;J22&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/99_Resources/Images/IDE_Blink.png", "Images/IDE_Blink.png"],</v>
       </c>
     </row>
@@ -5793,118 +5758,93 @@
         <v>291</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B23)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B23,C23,9999)</f>
         <v>ArduinoCode/03_YakityYak/README.md</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D23,"*.png*")+COUNTIF($D23,"*.jpg*")+COUNTIF($D23,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D23,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D23,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E23:G23),1,0)</f>
         <v>0</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E23+F23,MID(D23,1+FIND("/",D23),999),IF(G23&gt;0,SUBSTITUTE(SUBSTITUTE(D23,"/README.md",".html"),"/","_"),SUBSTITUTE(D23,"/","_")&amp;".html"))</f>
         <v>ArduinoCode_03_YakityYak.html</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="0"/>
+        <f>"    ["""&amp;B23&amp;""", """&amp;J23&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/ArduinoCode/03_YakityYak/README.md", "ArduinoCode_03_YakityYak.html"],</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>LEN(B24)</f>
-        <v>89</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="2"/>
-        <v>ArduinoCode/01_Blink/README.md</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="7"/>
-        <v>ArduinoCode_01_Blink.html</v>
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>309</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/01_Blink/README.md", "ArduinoCode_01_Blink.html"],</v>
+        <f>"    ["""&amp;B24&amp;""", """&amp;J24&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/01_Blink/01_Blink.ino", "ArduinoCode/01_Blink/01_Blink.ino"],</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>LEN(B25)</f>
-        <v>88</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>293</v>
+        <v>89</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>59</v>
+        <f>FIND("master/",B25)+LEN("master")+1</f>
+        <v>60</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="2"/>
-        <v>00_InstallArduinoIDE/README.md</v>
+        <f>MID(B25,C25,9999)</f>
+        <v>ArduinoCode/01_Blink/README.md</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D25,"*.png*")+COUNTIF($D25,"*.jpg*")+COUNTIF($D25,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D25,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G25">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D25,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H25">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E25:G25),1,0)</f>
         <v>0</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="7"/>
-        <v>00_InstallArduinoIDE.html</v>
+        <f>IF(E25+F25,MID(D25,1+FIND("/",D25),999),IF(G25&gt;0,SUBSTITUTE(SUBSTITUTE(D25,"/README.md",".html"),"/","_"),SUBSTITUTE(D25,"/","_")&amp;".html"))</f>
+        <v>ArduinoCode_01_Blink.html</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/00_InstallArduinoIDE/README.md", "00_InstallArduinoIDE.html"],</v>
+        <f>"    ["""&amp;B25&amp;""", """&amp;J25&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/ArduinoCode/01_Blink/README.md", "ArduinoCode_01_Blink.html"],</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5913,203 +5853,203 @@
         <v>88</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B26)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="2"/>
-        <v>ArduinoCode/01_Blink/README.md</v>
+        <f>MID(B26,C26,9999)</f>
+        <v>00_InstallArduinoIDE/README.md</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D26,"*.png*")+COUNTIF($D26,"*.jpg*")+COUNTIF($D26,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D26,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G26">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D26,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H26">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E26:G26),1,0)</f>
         <v>0</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="7"/>
-        <v>ArduinoCode_01_Blink.html</v>
+        <f>IF(E26+F26,MID(D26,1+FIND("/",D26),999),IF(G26&gt;0,SUBSTITUTE(SUBSTITUTE(D26,"/README.md",".html"),"/","_"),SUBSTITUTE(D26,"/","_")&amp;".html"))</f>
+        <v>00_InstallArduinoIDE.html</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/ArduinoCode/01_Blink/README.md", "ArduinoCode_01_Blink.html"],</v>
+        <f>"    ["""&amp;B26&amp;""", """&amp;J26&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/00_InstallArduinoIDE/README.md", "00_InstallArduinoIDE.html"],</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>LEN(B27)</f>
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B27)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="2"/>
-        <v>02_LetsGetTalking/README.md</v>
+        <f>MID(B27,C27,9999)</f>
+        <v>ArduinoCode/01_Blink/README.md</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D27,"*.png*")+COUNTIF($D27,"*.jpg*")+COUNTIF($D27,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D27,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D27,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H27">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E27:G27),1,0)</f>
         <v>0</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="7"/>
-        <v>02_LetsGetTalking.html</v>
+        <f>IF(E27+F27,MID(D27,1+FIND("/",D27),999),IF(G27&gt;0,SUBSTITUTE(SUBSTITUTE(D27,"/README.md",".html"),"/","_"),SUBSTITUTE(D27,"/","_")&amp;".html"))</f>
+        <v>ArduinoCode_01_Blink.html</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/02_LetsGetTalking/README.md", "02_LetsGetTalking.html"],</v>
+        <f>"    ["""&amp;B27&amp;""", """&amp;J27&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/ArduinoCode/01_Blink/README.md", "ArduinoCode_01_Blink.html"],</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>LEN(B28)</f>
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B28)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="2"/>
-        <v>01_BlinkingLED/README.md</v>
+        <f>MID(B28,C28,9999)</f>
+        <v>02_LetsGetTalking/README.md</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D28,"*.png*")+COUNTIF($D28,"*.jpg*")+COUNTIF($D28,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D28,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G28">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D28,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H28">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E28:G28),1,0)</f>
         <v>0</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="7"/>
-        <v>01_BlinkingLED.html</v>
+        <f>IF(E28+F28,MID(D28,1+FIND("/",D28),999),IF(G28&gt;0,SUBSTITUTE(SUBSTITUTE(D28,"/README.md",".html"),"/","_"),SUBSTITUTE(D28,"/","_")&amp;".html"))</f>
+        <v>02_LetsGetTalking.html</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/01_BlinkingLED/README.md", "01_BlinkingLED.html"],</v>
+        <f>"    ["""&amp;B28&amp;""", """&amp;J28&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/02_LetsGetTalking/README.md", "02_LetsGetTalking.html"],</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>LEN(B29)</f>
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B29)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="2"/>
-        <v>03_YakityYak/README.md</v>
+        <f>MID(B29,C29,9999)</f>
+        <v>01_BlinkingLED/README.md</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D29,"*.png*")+COUNTIF($D29,"*.jpg*")+COUNTIF($D29,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D29,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G29">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D29,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H29">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E29:G29),1,0)</f>
         <v>0</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="7"/>
-        <v>03_YakityYak.html</v>
+        <f>IF(E29+F29,MID(D29,1+FIND("/",D29),999),IF(G29&gt;0,SUBSTITUTE(SUBSTITUTE(D29,"/README.md",".html"),"/","_"),SUBSTITUTE(D29,"/","_")&amp;".html"))</f>
+        <v>01_BlinkingLED.html</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/03_YakityYak/README.md", "03_YakityYak.html"],</v>
+        <f>"    ["""&amp;B29&amp;""", """&amp;J29&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/01_BlinkingLED/README.md", "01_BlinkingLED.html"],</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>LEN(B30)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B30)+LEN("master")+1</f>
         <v>59</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="2"/>
-        <v>ArduinoCode/README.md</v>
+        <f>MID(B30,C30,9999)</f>
+        <v>03_YakityYak/README.md</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D30,"*.png*")+COUNTIF($D30,"*.jpg*")+COUNTIF($D30,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D30,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G30">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D30,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H30">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E30:G30),1,0)</f>
         <v>0</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="7"/>
-        <v>ArduinoCode.html</v>
+        <f>IF(E30+F30,MID(D30,1+FIND("/",D30),999),IF(G30&gt;0,SUBSTITUTE(SUBSTITUTE(D30,"/README.md",".html"),"/","_"),SUBSTITUTE(D30,"/","_")&amp;".html"))</f>
+        <v>03_YakityYak.html</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/ArduinoCode/README.md", "ArduinoCode.html"],</v>
+        <f>"    ["""&amp;B30&amp;""", """&amp;J30&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/03_YakityYak/README.md", "03_YakityYak.html"],</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -6118,371 +6058,416 @@
         <v>79</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f>FIND("master/",B31)+LEN("master")+1</f>
+        <v>59</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="2"/>
-        <v>00_InstallArduinoIDE</v>
+        <f>MID(B31,C31,9999)</f>
+        <v>ArduinoCode/README.md</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D31,"*.png*")+COUNTIF($D31,"*.jpg*")+COUNTIF($D31,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D31,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G31">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>IF(COUNTIF($D31,"*.md*"),1,0)</f>
+        <v>1</v>
       </c>
       <c r="H31">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>IF(0=SUM(E31:G31),1,0)</f>
+        <v>0</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="7"/>
-        <v>00_InstallArduinoIDE.html</v>
+        <f>IF(E31+F31,MID(D31,1+FIND("/",D31),999),IF(G31&gt;0,SUBSTITUTE(SUBSTITUTE(D31,"/README.md",".html"),"/","_"),SUBSTITUTE(D31,"/","_")&amp;".html"))</f>
+        <v>ArduinoCode.html</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/00_InstallArduinoIDE", "00_InstallArduinoIDE.html"],</v>
+        <f>"    ["""&amp;B31&amp;""", """&amp;J31&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/ArduinoCode/README.md", "ArduinoCode.html"],</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>LEN(B32)</f>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B32)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="2"/>
-        <v>02_LetsGetTalking</v>
+        <f>MID(B32,C32,9999)</f>
+        <v>00_InstallArduinoIDE</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D32,"*.png*")+COUNTIF($D32,"*.jpg*")+COUNTIF($D32,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D32,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G32">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D32,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H32">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E32:G32),1,0)</f>
         <v>1</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="7"/>
-        <v>02_LetsGetTalking.html</v>
+        <f>IF(E32+F32,MID(D32,1+FIND("/",D32),999),IF(G32&gt;0,SUBSTITUTE(SUBSTITUTE(D32,"/README.md",".html"),"/","_"),SUBSTITUTE(D32,"/","_")&amp;".html"))</f>
+        <v>00_InstallArduinoIDE.html</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/02_LetsGetTalking", "02_LetsGetTalking.html"],</v>
+        <f>"    ["""&amp;B32&amp;""", """&amp;J32&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/00_InstallArduinoIDE", "00_InstallArduinoIDE.html"],</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>LEN(B33)</f>
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B33)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="2"/>
-        <v>01_BlinkingLED</v>
+        <f>MID(B33,C33,9999)</f>
+        <v>02_LetsGetTalking</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D33,"*.png*")+COUNTIF($D33,"*.jpg*")+COUNTIF($D33,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D33,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G33">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D33,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H33">
-        <f t="shared" si="6"/>
+        <f>IF(0=SUM(E33:G33),1,0)</f>
         <v>1</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="7"/>
-        <v>01_BlinkingLED.html</v>
+        <f>IF(E33+F33,MID(D33,1+FIND("/",D33),999),IF(G33&gt;0,SUBSTITUTE(SUBSTITUTE(D33,"/README.md",".html"),"/","_"),SUBSTITUTE(D33,"/","_")&amp;".html"))</f>
+        <v>02_LetsGetTalking.html</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/01_BlinkingLED", "01_BlinkingLED.html"],</v>
+        <f>"    ["""&amp;B33&amp;""", """&amp;J33&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/02_LetsGetTalking", "02_LetsGetTalking.html"],</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>LEN(B34)</f>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B34)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="2"/>
-        <v>03_YakityYak</v>
+        <f>MID(B34,C34,9999)</f>
+        <v>01_BlinkingLED</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D34,"*.png*")+COUNTIF($D34,"*.jpg*")+COUNTIF($D34,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D34,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D34,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J34" t="str">
-        <f t="shared" si="7"/>
-        <v>03_YakityYak.html</v>
+        <f>IF(0=SUM(E34:G34),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J34" s="5" t="str">
+        <f>IF(E34+F34,MID(D34,1+FIND("/",D34),999),IF(G34&gt;0,SUBSTITUTE(SUBSTITUTE(D34,"/README.md",".html"),"/","_"),SUBSTITUTE(D34,"/","_")&amp;".html"))</f>
+        <v>01_BlinkingLED.html</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/03_YakityYak", "03_YakityYak.html"],</v>
+        <f>"    ["""&amp;B34&amp;""", """&amp;J34&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/01_BlinkingLED", "01_BlinkingLED.html"],</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>LEN(B35)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B35)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="2"/>
-        <v>ArduinoCode</v>
+        <f>MID(B35,C35,9999)</f>
+        <v>03_YakityYak</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D35,"*.png*")+COUNTIF($D35,"*.jpg*")+COUNTIF($D35,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D35,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G35">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D35,"*.md*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="H35">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J35" t="str">
-        <f t="shared" si="7"/>
-        <v>ArduinoCode.html</v>
+        <f>IF(0=SUM(E35:G35),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="5" t="str">
+        <f>IF(E35+F35,MID(D35,1+FIND("/",D35),999),IF(G35&gt;0,SUBSTITUTE(SUBSTITUTE(D35,"/README.md",".html"),"/","_"),SUBSTITUTE(D35,"/","_")&amp;".html"))</f>
+        <v>03_YakityYak.html</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/ArduinoCode", "ArduinoCode.html"],</v>
+        <f>"    ["""&amp;B35&amp;""", """&amp;J35&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/03_YakityYak", "03_YakityYak.html"],</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>LEN(B36)</f>
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f>FIND("master/",B36)+LEN("master")+1</f>
         <v>60</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="2"/>
-        <v>README.md</v>
+        <f>MID(B36,C36,9999)</f>
+        <v>ArduinoCode</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D36,"*.png*")+COUNTIF($D36,"*.jpg*")+COUNTIF($D36,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D36,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G36">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f>IF(COUNTIF($D36,"*.md*"),1,0)</f>
+        <v>0</v>
       </c>
       <c r="H36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>221</v>
+        <f>IF(0=SUM(E36:G36),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J36" s="5" t="str">
+        <f>IF(E36+F36,MID(D36,1+FIND("/",D36),999),IF(G36&gt;0,SUBSTITUTE(SUBSTITUTE(D36,"/README.md",".html"),"/","_"),SUBSTITUTE(D36,"/","_")&amp;".html"))</f>
+        <v>ArduinoCode.html</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/README.md", "_index.html"],</v>
+        <f>"    ["""&amp;B36&amp;""", """&amp;J36&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master/ArduinoCode", "ArduinoCode.html"],</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>LEN(B37)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>59</v>
+        <f>FIND("master/",B37)+LEN("master")+1</f>
+        <v>60</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="2"/>
+        <f>MID(B37,C37,9999)</f>
         <v>README.md</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D37,"*.png*")+COUNTIF($D37,"*.jpg*")+COUNTIF($D37,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D37,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G37">
-        <f t="shared" si="5"/>
+        <f>IF(COUNTIF($D37,"*.md*"),1,0)</f>
         <v>1</v>
       </c>
       <c r="H37">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="4" t="s">
+        <f>IF(0=SUM(E37:G37),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="7" t="s">
         <v>221</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/README.md", "_index.html"],</v>
+        <f>"    ["""&amp;B37&amp;""", """&amp;J37&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/blob/master/README.md", "_index.html"],</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>LEN(B38)</f>
-        <v>58</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C38" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D38" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>67</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C38">
+        <f>FIND("master/",B38)+LEN("master")+1</f>
+        <v>59</v>
+      </c>
+      <c r="D38" t="str">
+        <f>MID(B38,C38,9999)</f>
+        <v>README.md</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($D38,"*.png*")+COUNTIF($D38,"*.jpg*")+COUNTIF($D38,"*.pdf*")</f>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="4"/>
+        <f>IF(COUNTIF($D38,"*.xls*"),1,0)</f>
         <v>0</v>
       </c>
       <c r="G38">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>IF(COUNTIF($D38,"*.md*"),1,0)</f>
+        <v>1</v>
       </c>
       <c r="H38">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J38" s="4" t="s">
+        <f>IF(0=SUM(E38:G38),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>221</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master", "_index.html"],</v>
+        <f>"    ["""&amp;B38&amp;""", """&amp;J38&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/raw/master/README.md", "_index.html"],</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>LEN(B39)</f>
+        <v>58</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C39" t="e">
+        <f>FIND("master/",B39)+LEN("master")+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D39" t="e">
+        <f>MID(B39,C39,9999)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E39">
+        <f>COUNTIF($D39,"*.png*")+COUNTIF($D39,"*.jpg*")+COUNTIF($D39,"*.pdf*")</f>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>IF(COUNTIF($D39,"*.xls*"),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f>IF(COUNTIF($D39,"*.md*"),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <f>IF(0=SUM(E39:G39),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="K39" t="str">
+        <f>"    ["""&amp;B39&amp;""", """&amp;J39&amp;"""],"</f>
+        <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass/tree/master", "_index.html"],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>LEN(B40)</f>
         <v>46</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C39" t="e">
-        <f t="shared" si="1"/>
+      <c r="C40" t="e">
+        <f>FIND("master/",B40)+LEN("master")+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D39" t="e">
-        <f t="shared" si="2"/>
+      <c r="D40" t="e">
+        <f>MID(B40,C40,9999)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="J39" s="4" t="s">
+      <c r="E40">
+        <f>COUNTIF($D40,"*.png*")+COUNTIF($D40,"*.jpg*")+COUNTIF($D40,"*.pdf*")</f>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f>IF(COUNTIF($D40,"*.xls*"),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f>IF(COUNTIF($D40,"*.md*"),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <f>IF(0=SUM(E40:G40),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J40" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="K39" t="str">
-        <f t="shared" si="0"/>
+      <c r="K40" t="str">
+        <f>"    ["""&amp;B40&amp;""", """&amp;J40&amp;"""],"</f>
         <v xml:space="preserve">    ["https://github.com/Mark-MDO47/CforArduinoClass", "_index.html"],</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K40">
+    <sortCondition descending="1" ref="A3:A40"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B38" r:id="rId1" xr:uid="{79CE2A96-0584-4CAD-8E78-0EA8BEE8845A}"/>
-    <hyperlink ref="B39" r:id="rId2" xr:uid="{C5459398-9BDC-4B0E-9D81-49D417C3A08F}"/>
+    <hyperlink ref="B39" r:id="rId1" xr:uid="{79CE2A96-0584-4CAD-8E78-0EA8BEE8845A}"/>
+    <hyperlink ref="B40" r:id="rId2" xr:uid="{C5459398-9BDC-4B0E-9D81-49D417C3A08F}"/>
+    <hyperlink ref="B25" r:id="rId3" xr:uid="{82D2EF0B-20AF-4645-B2C3-DF46A7719767}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>